<commit_message>
finished functional part of q1
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -14,12 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Inputs</t>
   </si>
   <si>
-    <t>lambda</t>
+    <t>Desired P(block)</t>
+  </si>
+  <si>
+    <t>Arrival Rate</t>
+  </si>
+  <si>
+    <t>Service Rate</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Number of Servers</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Actual P(block)</t>
+  </si>
+  <si>
+    <t>0.008747498215510364</t>
   </si>
 </sst>
 </file>
@@ -351,20 +384,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
q2 almost done, change E(w) to conditional
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Part 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,25 +19,31 @@
     <t>Inputs</t>
   </si>
   <si>
-    <t>Desired P(block)</t>
-  </si>
-  <si>
     <t>Arrival Rate</t>
   </si>
   <si>
     <t>Service Rate</t>
   </si>
   <si>
+    <t>P(W &gt; 0) Less Than</t>
+  </si>
+  <si>
+    <t>E(W) Less Than</t>
+  </si>
+  <si>
     <t>Values</t>
   </si>
   <si>
-    <t>0.01</t>
-  </si>
-  <si>
     <t>10.0</t>
   </si>
   <si>
-    <t>12.0</t>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.25</t>
   </si>
   <si>
     <t>Results</t>
@@ -46,13 +52,7 @@
     <t>Number of Servers</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Actual P(block)</t>
-  </si>
-  <si>
-    <t>0.008747498215510364</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +395,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -403,7 +403,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -419,27 +419,27 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ew --> ew | p(w > 0), and --> or, working??
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -43,7 +43,7 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>0.25</t>
+    <t>0.5</t>
   </si>
   <si>
     <t>Results</t>
@@ -52,7 +52,7 @@
     <t>Number of Servers</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
gui working for erlang b, change structure
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Part 2" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,31 +19,25 @@
     <t>Inputs</t>
   </si>
   <si>
+    <t>Desired P(block)</t>
+  </si>
+  <si>
     <t>Arrival Rate</t>
   </si>
   <si>
     <t>Service Rate</t>
   </si>
   <si>
-    <t>P(W &gt; 0) Less Than</t>
-  </si>
-  <si>
-    <t>E(W) Less Than</t>
-  </si>
-  <si>
     <t>Values</t>
   </si>
   <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
     <t>0.2</t>
   </si>
   <si>
-    <t>0.5</t>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>6.0</t>
   </si>
   <si>
     <t>Results</t>
@@ -52,7 +46,13 @@
     <t>Number of Servers</t>
   </si>
   <si>
-    <t>3</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Actual P(block)</t>
+  </si>
+  <si>
+    <t>0.1592356687898089</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +395,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -403,7 +403,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -419,27 +419,27 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
erlang-c part of menu
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -7,37 +7,43 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Part 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Inputs</t>
   </si>
   <si>
-    <t>Desired P(block)</t>
-  </si>
-  <si>
     <t>Arrival Rate</t>
   </si>
   <si>
     <t>Service Rate</t>
   </si>
   <si>
+    <t>P(W &gt; 0) Less Than</t>
+  </si>
+  <si>
+    <t>E(W) Less Than</t>
+  </si>
+  <si>
     <t>Values</t>
   </si>
   <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
     <t>0.2</t>
   </si>
   <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>6.0</t>
+    <t>0.5</t>
   </si>
   <si>
     <t>Results</t>
@@ -46,13 +52,19 @@
     <t>Number of Servers</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Actual P(block)</t>
-  </si>
-  <si>
-    <t>0.1592356687898089</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>E(S)</t>
+  </si>
+  <si>
+    <t>0.05555555555555556</t>
+  </si>
+  <si>
+    <t>E(N)</t>
+  </si>
+  <si>
+    <t>0.38461538461538464</t>
   </si>
 </sst>
 </file>
@@ -384,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -403,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -411,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -419,28 +431,44 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compile to windows dll
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -7,37 +7,43 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Part 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Inputs</t>
   </si>
   <si>
-    <t>Desired P(block)</t>
-  </si>
-  <si>
     <t>Arrival Rate</t>
   </si>
   <si>
     <t>Service Rate</t>
   </si>
   <si>
+    <t>P(W &gt; 0) Less Than</t>
+  </si>
+  <si>
+    <t>E(W) Less Than</t>
+  </si>
+  <si>
     <t>Values</t>
   </si>
   <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>101.0</t>
+  </si>
+  <si>
     <t>0.2</t>
   </si>
   <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>6.0</t>
+    <t>1.0</t>
   </si>
   <si>
     <t>Results</t>
@@ -46,13 +52,19 @@
     <t>Number of Servers</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Actual P(block)</t>
-  </si>
-  <si>
-    <t>0.1592356687898089</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>E(S)</t>
+  </si>
+  <si>
+    <t>0.0033003300330033004</t>
+  </si>
+  <si>
+    <t>E(N)</t>
+  </si>
+  <si>
+    <t>0.49261083743842365</t>
   </si>
 </sst>
 </file>
@@ -384,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -403,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -411,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -419,28 +431,44 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed all but p2
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -422,7 +422,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -432,7 +432,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
     </row>
@@ -444,7 +444,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -454,7 +454,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.15094339622641512</t>
+          <t>0.0006416879652056608</t>
         </is>
       </c>
     </row>
@@ -469,8 +469,6 @@
           <t>5.0</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -483,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,52 +500,92 @@
           <t>Values</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Results</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arrival Rate</t>
+          <t>Max P(wait)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Number of Servers</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Service Rate</t>
+          <t>Max E(w)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>101.0</t>
+          <t>30.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>E(S)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.02380952380952381</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P(W &gt; 0) Less Than</t>
+          <t>Arrival Rate</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>E(N)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.02380952380952381</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E(W) Less Than</t>
+          <t>Service Rate</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>21.0</t>
         </is>
       </c>
     </row>
@@ -643,7 +681,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -653,7 +691,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.6701030927835052</t>
         </is>
       </c>
     </row>
@@ -665,7 +703,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -675,7 +713,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>89.99999999999997</t>
+          <t>1.8556701030927834</t>
         </is>
       </c>
     </row>
@@ -687,7 +725,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -697,7 +735,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.011111111111111115</t>
+          <t>0.538888888888889</t>
         </is>
       </c>
     </row>
@@ -709,7 +747,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.9988888888888889</t>
+          <t>0.32638888888888884</t>
         </is>
       </c>
     </row>
@@ -762,7 +800,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>40.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -772,7 +810,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.7999087254067538</t>
+          <t>0.6780485778822252</t>
         </is>
       </c>
     </row>
@@ -784,7 +822,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -794,7 +832,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3.081135750457513</t>
+          <t>1.5243927764721845</t>
         </is>
       </c>
     </row>
@@ -806,7 +844,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
@@ -859,7 +897,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -869,7 +907,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.6536161131250601</t>
+          <t>1.051948051948052</t>
         </is>
       </c>
     </row>
@@ -881,7 +919,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>52.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -891,7 +929,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.34638388687493993</t>
+          <t>-0.051948051948051965</t>
         </is>
       </c>
     </row>
@@ -903,7 +941,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>51.0</t>
+          <t>4.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed p2, TODO es->ew, implement other requests in prompt
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.02380952380952381</t>
+          <t>0.06666666666666667</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.02380952380952381</t>
+          <t>1.9999999999999998</t>
         </is>
       </c>
     </row>
@@ -585,9 +585,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21.0</t>
-        </is>
-      </c>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">

</xml_diff>

<commit_message>
fixed p2 and p5
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -551,7 +551,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>0.017391304347826087</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.051948051948052</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-0.051948051948051965</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>7.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change EN calculation, split erlang c into two programs
</commit_message>
<xml_diff>
--- a/queuing_theory.xlsx
+++ b/queuing_theory.xlsx
@@ -422,7 +422,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>0.005</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -432,7 +432,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
     </row>
@@ -444,7 +444,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>1.75</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -454,7 +454,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0006416879652056608</t>
+          <t>0.0033186086434399764</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>0.25</t>
         </is>
       </c>
     </row>
@@ -517,11 +517,7 @@
           <t>Max P(wait)</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>Number of Servers</t>
@@ -551,7 +547,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.017391304347826087</t>
+          <t>0.1018867924528302</t>
         </is>
       </c>
     </row>
@@ -563,7 +559,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -573,7 +569,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.528301886792453</t>
         </is>
       </c>
     </row>
@@ -683,7 +679,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>30.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -693,7 +689,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.6701030927835052</t>
+          <t>0.8196836008567772</t>
         </is>
       </c>
     </row>
@@ -705,7 +701,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -715,7 +711,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.8556701030927834</t>
+          <t>81.14237961445023</t>
         </is>
       </c>
     </row>
@@ -727,7 +723,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -737,7 +733,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.538888888888889</t>
+          <t>0.012324016189216061</t>
         </is>
       </c>
     </row>
@@ -749,7 +745,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.32638888888888884</t>
+          <t>0.9753519676215678</t>
         </is>
       </c>
     </row>
@@ -802,7 +798,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -812,7 +808,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.6780485778822252</t>
+          <t>0.6893203883495146</t>
         </is>
       </c>
     </row>
@@ -824,7 +820,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -834,7 +830,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.5243927764721845</t>
+          <t>1.2427184466019416</t>
         </is>
       </c>
     </row>
@@ -846,7 +842,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>20.0</t>
         </is>
       </c>
     </row>
@@ -899,7 +895,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -909,7 +905,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5294117647058824</t>
         </is>
       </c>
     </row>
@@ -921,7 +917,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -931,7 +927,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.47058823529411764</t>
         </is>
       </c>
     </row>
@@ -943,7 +939,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>

</xml_diff>